<commit_message>
CO PO Mapping DCC CO4I Unit Test 1, PA,MicroProject Marks added
</commit_message>
<xml_diff>
--- a/CO PO Mapping/DCC/Criteria 3_PO attain_DCC_CO3I_19-20_CO_GRWPL.xlsx
+++ b/CO PO Mapping/DCC/Criteria 3_PO attain_DCC_CO3I_19-20_CO_GRWPL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="15600" windowHeight="7875" tabRatio="715" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="15600" windowHeight="7875" tabRatio="715"/>
   </bookViews>
   <sheets>
     <sheet name="PO Set Target attain level" sheetId="12" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="273">
   <si>
     <t>Course Name :</t>
   </si>
@@ -3384,6 +3384,37 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4183,37 +4214,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4535,8 +4535,8 @@
   </sheetPr>
   <dimension ref="B1:N29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4611,50 +4611,50 @@
       <c r="C8" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="309" t="s">
+      <c r="D8" s="317" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="310"/>
+      <c r="E8" s="318"/>
     </row>
     <row r="9" spans="2:13" ht="35.25" customHeight="1">
       <c r="B9" s="137"/>
       <c r="C9" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="309" t="s">
+      <c r="D9" s="317" t="s">
         <v>268</v>
       </c>
-      <c r="E9" s="310"/>
+      <c r="E9" s="318"/>
     </row>
     <row r="10" spans="2:13" ht="32.25" customHeight="1">
       <c r="B10" s="137"/>
       <c r="C10" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="309" t="s">
+      <c r="D10" s="317" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="310"/>
+      <c r="E10" s="318"/>
     </row>
     <row r="11" spans="2:13" ht="28.5" customHeight="1">
       <c r="B11" s="137"/>
       <c r="C11" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="309" t="s">
+      <c r="D11" s="317" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="310"/>
+      <c r="E11" s="318"/>
     </row>
     <row r="12" spans="2:13" ht="27.75" customHeight="1">
       <c r="B12" s="137"/>
       <c r="C12" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="309" t="s">
+      <c r="D12" s="317" t="s">
         <v>271</v>
       </c>
-      <c r="E12" s="310"/>
+      <c r="E12" s="318"/>
     </row>
     <row r="14" spans="2:13" ht="18.75">
       <c r="B14" s="115" t="s">
@@ -4689,31 +4689,31 @@
       <c r="M15" s="114"/>
     </row>
     <row r="16" spans="2:13" ht="16.5" thickBot="1">
-      <c r="B16" s="311" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="314" t="s">
+      <c r="B16" s="319" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="322" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="315"/>
-      <c r="E16" s="320" t="s">
+      <c r="D16" s="323"/>
+      <c r="E16" s="328" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="321"/>
-      <c r="G16" s="321"/>
-      <c r="H16" s="321"/>
-      <c r="I16" s="321"/>
-      <c r="J16" s="321"/>
-      <c r="K16" s="322"/>
-      <c r="L16" s="320" t="s">
+      <c r="F16" s="329"/>
+      <c r="G16" s="329"/>
+      <c r="H16" s="329"/>
+      <c r="I16" s="329"/>
+      <c r="J16" s="329"/>
+      <c r="K16" s="330"/>
+      <c r="L16" s="328" t="s">
         <v>97</v>
       </c>
-      <c r="M16" s="321"/>
+      <c r="M16" s="329"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B17" s="312"/>
-      <c r="C17" s="316"/>
-      <c r="D17" s="317"/>
+      <c r="B17" s="320"/>
+      <c r="C17" s="324"/>
+      <c r="D17" s="325"/>
       <c r="E17" s="118" t="s">
         <v>98</v>
       </c>
@@ -4743,9 +4743,9 @@
       </c>
     </row>
     <row r="18" spans="2:14" ht="88.5" customHeight="1" thickBot="1">
-      <c r="B18" s="313"/>
-      <c r="C18" s="318"/>
-      <c r="D18" s="319"/>
+      <c r="B18" s="321"/>
+      <c r="C18" s="326"/>
+      <c r="D18" s="327"/>
       <c r="E18" s="119" t="s">
         <v>133</v>
       </c>
@@ -4787,13 +4787,13 @@
         <v>Analyze the functioning of data communication and computer network</v>
       </c>
       <c r="E19" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19" s="125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" s="125">
         <v>1</v>
@@ -4802,16 +4802,16 @@
         <v>187</v>
       </c>
       <c r="J19" s="229">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L19" s="125">
-        <v>2</v>
-      </c>
-      <c r="M19" s="125" t="s">
-        <v>187</v>
+        <v>1</v>
+      </c>
+      <c r="M19" s="125">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="24.75" thickBot="1">
@@ -4827,31 +4827,31 @@
         <v>Select relavant transmission media and switching techniques as per need</v>
       </c>
       <c r="E20" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="125">
-        <v>2</v>
-      </c>
-      <c r="I20" s="125">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I20" s="125" t="s">
+        <v>187</v>
       </c>
       <c r="J20" s="229">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L20" s="125">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" s="125">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="27.75" customHeight="1" thickBot="1">
@@ -4867,16 +4867,16 @@
         <v>Analyze the transmission errors with respect to IEEE standards</v>
       </c>
       <c r="E21" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="125">
         <v>2</v>
       </c>
       <c r="G21" s="125">
-        <v>3</v>
-      </c>
-      <c r="H21" s="125" t="s">
-        <v>187</v>
+        <v>2</v>
+      </c>
+      <c r="H21" s="125">
+        <v>1</v>
       </c>
       <c r="I21" s="125">
         <v>1</v>
@@ -4885,13 +4885,13 @@
         <v>3</v>
       </c>
       <c r="K21" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L21" s="125">
-        <v>1</v>
-      </c>
-      <c r="M21" s="125" t="s">
-        <v>187</v>
+        <v>2</v>
+      </c>
+      <c r="M21" s="125">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1">
@@ -4913,25 +4913,25 @@
         <v>2</v>
       </c>
       <c r="G22" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" s="125">
         <v>2</v>
       </c>
-      <c r="I22" s="125">
-        <v>1</v>
+      <c r="I22" s="125" t="s">
+        <v>187</v>
       </c>
       <c r="J22" s="125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K22" s="125">
         <v>3</v>
       </c>
       <c r="L22" s="125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M22" s="125">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="26.25" customHeight="1" thickBot="1">
@@ -4947,58 +4947,58 @@
         <v>Configure different TCP/IP Services</v>
       </c>
       <c r="E23" s="125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" s="125">
         <v>2</v>
       </c>
       <c r="H23" s="125">
+        <v>2</v>
+      </c>
+      <c r="I23" s="125">
         <v>1</v>
       </c>
-      <c r="I23" s="125">
-        <v>2</v>
-      </c>
       <c r="J23" s="229">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K23" s="125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" s="125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M23" s="125">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B24" s="306" t="s">
+      <c r="B24" s="314" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="307"/>
-      <c r="D24" s="308"/>
+      <c r="C24" s="315"/>
+      <c r="D24" s="316"/>
       <c r="E24" s="127">
         <f t="shared" ref="E24:K24" si="1">ROUNDUP(AVERAGE(E19:E23),2)</f>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="F24" s="127">
         <f t="shared" si="1"/>
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
       <c r="G24" s="127">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>1.8</v>
       </c>
       <c r="H24" s="127">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="I24" s="127">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J24" s="127">
         <f t="shared" si="1"/>
@@ -5006,15 +5006,15 @@
       </c>
       <c r="K24" s="127">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="L24" s="127">
         <f>IFERROR(ROUNDUP(AVERAGE(L19:L23),2),"-")</f>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M24" s="127">
         <f>ROUNDUP(AVERAGE(M19:M23),2)</f>
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="N24" s="257"/>
     </row>
@@ -5055,7 +5055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
@@ -6022,8 +6022,8 @@
   </sheetPr>
   <dimension ref="A1:BI110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="AD79" sqref="AD79"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6093,55 +6093,55 @@
     </row>
     <row r="7" spans="1:61" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:61" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A8" s="392" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="390" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="390" t="s">
+      <c r="A8" s="400" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="398" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="398" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="390" t="s">
+      <c r="D8" s="398" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="390"/>
-      <c r="F8" s="390"/>
-      <c r="G8" s="390"/>
-      <c r="H8" s="390"/>
-      <c r="I8" s="390"/>
-      <c r="J8" s="390"/>
-      <c r="K8" s="390"/>
-      <c r="L8" s="390"/>
+      <c r="E8" s="398"/>
+      <c r="F8" s="398"/>
+      <c r="G8" s="398"/>
+      <c r="H8" s="398"/>
+      <c r="I8" s="398"/>
+      <c r="J8" s="398"/>
+      <c r="K8" s="398"/>
+      <c r="L8" s="398"/>
       <c r="M8" s="270"/>
-      <c r="N8" s="390" t="s">
+      <c r="N8" s="398" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="390"/>
-      <c r="P8" s="390"/>
-      <c r="Q8" s="390"/>
-      <c r="R8" s="390"/>
-      <c r="S8" s="390"/>
-      <c r="T8" s="390"/>
-      <c r="U8" s="390"/>
-      <c r="V8" s="390"/>
-      <c r="W8" s="390"/>
-      <c r="X8" s="363" t="s">
+      <c r="O8" s="398"/>
+      <c r="P8" s="398"/>
+      <c r="Q8" s="398"/>
+      <c r="R8" s="398"/>
+      <c r="S8" s="398"/>
+      <c r="T8" s="398"/>
+      <c r="U8" s="398"/>
+      <c r="V8" s="398"/>
+      <c r="W8" s="398"/>
+      <c r="X8" s="371" t="s">
         <v>14</v>
       </c>
-      <c r="Y8" s="366" t="s">
+      <c r="Y8" s="374" t="s">
         <v>22</v>
       </c>
-      <c r="Z8" s="371" t="s">
+      <c r="Z8" s="379" t="s">
         <v>15</v>
       </c>
-      <c r="AA8" s="373" t="s">
+      <c r="AA8" s="381" t="s">
         <v>16</v>
       </c>
-      <c r="AB8" s="375" t="s">
+      <c r="AB8" s="383" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="377" t="s">
+      <c r="AC8" s="385" t="s">
         <v>18</v>
       </c>
       <c r="AD8" s="172" t="s">
@@ -6182,47 +6182,47 @@
       <c r="BI8" s="21"/>
     </row>
     <row r="9" spans="1:61" s="5" customFormat="1" ht="18.95" customHeight="1" thickBot="1">
-      <c r="A9" s="392"/>
-      <c r="B9" s="390"/>
-      <c r="C9" s="390"/>
-      <c r="D9" s="391" t="s">
+      <c r="A9" s="400"/>
+      <c r="B9" s="398"/>
+      <c r="C9" s="398"/>
+      <c r="D9" s="399" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="391"/>
-      <c r="F9" s="391"/>
-      <c r="G9" s="391"/>
-      <c r="H9" s="391"/>
-      <c r="I9" s="391"/>
-      <c r="J9" s="391" t="s">
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
+      <c r="G9" s="399"/>
+      <c r="H9" s="399"/>
+      <c r="I9" s="399"/>
+      <c r="J9" s="399" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="391"/>
-      <c r="L9" s="391"/>
+      <c r="K9" s="399"/>
+      <c r="L9" s="399"/>
       <c r="M9" s="271"/>
-      <c r="N9" s="391" t="s">
+      <c r="N9" s="399" t="s">
         <v>5</v>
       </c>
-      <c r="O9" s="391"/>
-      <c r="P9" s="391"/>
-      <c r="Q9" s="391"/>
-      <c r="R9" s="391"/>
-      <c r="S9" s="391" t="s">
+      <c r="O9" s="399"/>
+      <c r="P9" s="399"/>
+      <c r="Q9" s="399"/>
+      <c r="R9" s="399"/>
+      <c r="S9" s="399" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="391"/>
-      <c r="U9" s="391"/>
-      <c r="V9" s="391"/>
-      <c r="W9" s="391"/>
-      <c r="X9" s="364"/>
-      <c r="Y9" s="367"/>
-      <c r="Z9" s="372"/>
-      <c r="AA9" s="374"/>
-      <c r="AB9" s="376"/>
-      <c r="AC9" s="378"/>
-      <c r="AD9" s="341" t="s">
+      <c r="T9" s="399"/>
+      <c r="U9" s="399"/>
+      <c r="V9" s="399"/>
+      <c r="W9" s="399"/>
+      <c r="X9" s="372"/>
+      <c r="Y9" s="375"/>
+      <c r="Z9" s="380"/>
+      <c r="AA9" s="382"/>
+      <c r="AB9" s="384"/>
+      <c r="AC9" s="386"/>
+      <c r="AD9" s="349" t="s">
         <v>20</v>
       </c>
-      <c r="AE9" s="342"/>
+      <c r="AE9" s="350"/>
       <c r="AF9" s="21"/>
       <c r="AG9" s="21"/>
       <c r="AH9" s="21"/>
@@ -6255,9 +6255,9 @@
       <c r="BI9" s="21"/>
     </row>
     <row r="10" spans="1:61" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A10" s="392"/>
-      <c r="B10" s="390"/>
-      <c r="C10" s="390"/>
+      <c r="A10" s="400"/>
+      <c r="B10" s="398"/>
+      <c r="C10" s="398"/>
       <c r="D10" s="301" t="s">
         <v>6</v>
       </c>
@@ -6318,14 +6318,14 @@
       <c r="W10" s="274" t="s">
         <v>10</v>
       </c>
-      <c r="X10" s="364"/>
-      <c r="Y10" s="367"/>
-      <c r="Z10" s="372"/>
-      <c r="AA10" s="374"/>
-      <c r="AB10" s="376"/>
-      <c r="AC10" s="378"/>
-      <c r="AD10" s="341"/>
-      <c r="AE10" s="342"/>
+      <c r="X10" s="372"/>
+      <c r="Y10" s="375"/>
+      <c r="Z10" s="380"/>
+      <c r="AA10" s="382"/>
+      <c r="AB10" s="384"/>
+      <c r="AC10" s="386"/>
+      <c r="AD10" s="349"/>
+      <c r="AE10" s="350"/>
       <c r="AF10" s="21"/>
       <c r="AG10" s="21"/>
       <c r="AH10" s="21"/>
@@ -6358,9 +6358,9 @@
       <c r="BI10" s="21"/>
     </row>
     <row r="11" spans="1:61" s="5" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A11" s="392"/>
-      <c r="B11" s="390"/>
-      <c r="C11" s="390"/>
+      <c r="A11" s="400"/>
+      <c r="B11" s="398"/>
+      <c r="C11" s="398"/>
       <c r="D11" s="296" t="s">
         <v>41</v>
       </c>
@@ -6419,14 +6419,14 @@
         <v>41</v>
       </c>
       <c r="W11" s="272"/>
-      <c r="X11" s="365"/>
-      <c r="Y11" s="367"/>
-      <c r="Z11" s="372"/>
-      <c r="AA11" s="374"/>
-      <c r="AB11" s="376"/>
-      <c r="AC11" s="379"/>
-      <c r="AD11" s="341"/>
-      <c r="AE11" s="343"/>
+      <c r="X11" s="373"/>
+      <c r="Y11" s="375"/>
+      <c r="Z11" s="380"/>
+      <c r="AA11" s="382"/>
+      <c r="AB11" s="384"/>
+      <c r="AC11" s="387"/>
+      <c r="AD11" s="349"/>
+      <c r="AE11" s="351"/>
       <c r="AF11" s="21"/>
       <c r="AG11" s="21"/>
       <c r="AH11" s="21"/>
@@ -6459,9 +6459,9 @@
       <c r="BI11" s="21"/>
     </row>
     <row r="12" spans="1:61" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A12" s="392"/>
-      <c r="B12" s="390"/>
-      <c r="C12" s="390"/>
+      <c r="A12" s="400"/>
+      <c r="B12" s="398"/>
+      <c r="C12" s="398"/>
       <c r="D12" s="289">
         <v>2</v>
       </c>
@@ -7695,19 +7695,19 @@
       <c r="B29" s="252">
         <v>1801360227</v>
       </c>
-      <c r="C29" s="532" t="s">
+      <c r="C29" s="312" t="s">
         <v>259</v>
       </c>
-      <c r="D29" s="526"/>
-      <c r="E29" s="527"/>
-      <c r="F29" s="527"/>
-      <c r="G29" s="528"/>
-      <c r="H29" s="529"/>
-      <c r="I29" s="530"/>
-      <c r="J29" s="527"/>
-      <c r="K29" s="527"/>
-      <c r="L29" s="527"/>
-      <c r="M29" s="527"/>
+      <c r="D29" s="306"/>
+      <c r="E29" s="307"/>
+      <c r="F29" s="307"/>
+      <c r="G29" s="308"/>
+      <c r="H29" s="309"/>
+      <c r="I29" s="310"/>
+      <c r="J29" s="307"/>
+      <c r="K29" s="307"/>
+      <c r="L29" s="307"/>
+      <c r="M29" s="307"/>
       <c r="N29" s="34"/>
       <c r="O29" s="215"/>
       <c r="P29" s="215"/>
@@ -7736,7 +7736,7 @@
         <v>0</v>
       </c>
       <c r="AC29" s="228"/>
-      <c r="AD29" s="533" t="s">
+      <c r="AD29" s="313" t="s">
         <v>272</v>
       </c>
       <c r="AE29" s="11"/>
@@ -10709,16 +10709,16 @@
       <c r="C73" s="253" t="s">
         <v>261</v>
       </c>
-      <c r="D73" s="531"/>
-      <c r="E73" s="531"/>
-      <c r="F73" s="531"/>
-      <c r="G73" s="531"/>
-      <c r="H73" s="531"/>
-      <c r="I73" s="531"/>
-      <c r="J73" s="531"/>
-      <c r="K73" s="531"/>
-      <c r="L73" s="527"/>
-      <c r="M73" s="527"/>
+      <c r="D73" s="311"/>
+      <c r="E73" s="311"/>
+      <c r="F73" s="311"/>
+      <c r="G73" s="311"/>
+      <c r="H73" s="311"/>
+      <c r="I73" s="311"/>
+      <c r="J73" s="311"/>
+      <c r="K73" s="311"/>
+      <c r="L73" s="307"/>
+      <c r="M73" s="307"/>
       <c r="N73" s="34"/>
       <c r="O73" s="215"/>
       <c r="P73" s="215"/>
@@ -10747,7 +10747,7 @@
         <v>0</v>
       </c>
       <c r="AC73" s="228"/>
-      <c r="AD73" s="533" t="s">
+      <c r="AD73" s="313" t="s">
         <v>272</v>
       </c>
       <c r="AE73" s="11"/>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="AC77" s="228"/>
       <c r="AD77" s="281">
-        <f t="shared" ref="AD77:AD78" si="9">X77+Y77+AA77+AB77</f>
+        <f t="shared" ref="AD77" si="9">X77+Y77+AA77+AB77</f>
         <v>5</v>
       </c>
       <c r="AE77" s="133"/>
@@ -11022,16 +11022,16 @@
       <c r="C78" s="253" t="s">
         <v>258</v>
       </c>
-      <c r="D78" s="526"/>
-      <c r="E78" s="527"/>
-      <c r="F78" s="527"/>
-      <c r="G78" s="528"/>
-      <c r="H78" s="529"/>
-      <c r="I78" s="530"/>
-      <c r="J78" s="527"/>
-      <c r="K78" s="527"/>
-      <c r="L78" s="527"/>
-      <c r="M78" s="527"/>
+      <c r="D78" s="306"/>
+      <c r="E78" s="307"/>
+      <c r="F78" s="307"/>
+      <c r="G78" s="308"/>
+      <c r="H78" s="309"/>
+      <c r="I78" s="310"/>
+      <c r="J78" s="307"/>
+      <c r="K78" s="307"/>
+      <c r="L78" s="307"/>
+      <c r="M78" s="307"/>
       <c r="N78" s="34"/>
       <c r="O78" s="215"/>
       <c r="P78" s="215"/>
@@ -11060,7 +11060,7 @@
         <v>0</v>
       </c>
       <c r="AC78" s="228"/>
-      <c r="AD78" s="533" t="s">
+      <c r="AD78" s="313" t="s">
         <v>272</v>
       </c>
       <c r="AE78" s="261"/>
@@ -11266,158 +11266,158 @@
     <row r="85" spans="1:31" ht="15" customHeight="1" thickBot="1">
       <c r="A85" s="13"/>
       <c r="M85" s="198"/>
-      <c r="N85" s="380" t="s">
+      <c r="N85" s="388" t="s">
         <v>33</v>
       </c>
-      <c r="O85" s="381"/>
-      <c r="P85" s="381"/>
-      <c r="Q85" s="381"/>
-      <c r="R85" s="381"/>
-      <c r="S85" s="381"/>
-      <c r="T85" s="381"/>
-      <c r="U85" s="381"/>
-      <c r="V85" s="381"/>
-      <c r="W85" s="382"/>
-      <c r="X85" s="383">
+      <c r="O85" s="389"/>
+      <c r="P85" s="389"/>
+      <c r="Q85" s="389"/>
+      <c r="R85" s="389"/>
+      <c r="S85" s="389"/>
+      <c r="T85" s="389"/>
+      <c r="U85" s="389"/>
+      <c r="V85" s="389"/>
+      <c r="W85" s="390"/>
+      <c r="X85" s="391">
         <f t="shared" ref="X85:AC85" si="10">0.4*X12</f>
         <v>3.2</v>
       </c>
-      <c r="Y85" s="385">
+      <c r="Y85" s="393">
         <f t="shared" si="10"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="Z85" s="387">
+      <c r="Z85" s="395">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA85" s="389">
+      <c r="AA85" s="397">
         <f t="shared" si="10"/>
         <v>1.6</v>
       </c>
-      <c r="AB85" s="369">
+      <c r="AB85" s="377">
         <f t="shared" si="10"/>
         <v>0.8</v>
       </c>
-      <c r="AC85" s="370">
+      <c r="AC85" s="378">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD85" s="368"/>
-      <c r="AE85" s="368"/>
+      <c r="AD85" s="376"/>
+      <c r="AE85" s="376"/>
     </row>
     <row r="86" spans="1:31" ht="8.25" customHeight="1" thickBot="1">
       <c r="A86" s="13"/>
-      <c r="N86" s="380"/>
-      <c r="O86" s="381"/>
-      <c r="P86" s="381"/>
-      <c r="Q86" s="381"/>
-      <c r="R86" s="381"/>
-      <c r="S86" s="381"/>
-      <c r="T86" s="381"/>
-      <c r="U86" s="381"/>
-      <c r="V86" s="381"/>
-      <c r="W86" s="382"/>
-      <c r="X86" s="384"/>
-      <c r="Y86" s="386"/>
-      <c r="Z86" s="388"/>
-      <c r="AA86" s="351"/>
-      <c r="AB86" s="353"/>
-      <c r="AC86" s="355"/>
-      <c r="AD86" s="356"/>
-      <c r="AE86" s="356"/>
+      <c r="N86" s="388"/>
+      <c r="O86" s="389"/>
+      <c r="P86" s="389"/>
+      <c r="Q86" s="389"/>
+      <c r="R86" s="389"/>
+      <c r="S86" s="389"/>
+      <c r="T86" s="389"/>
+      <c r="U86" s="389"/>
+      <c r="V86" s="389"/>
+      <c r="W86" s="390"/>
+      <c r="X86" s="392"/>
+      <c r="Y86" s="394"/>
+      <c r="Z86" s="396"/>
+      <c r="AA86" s="359"/>
+      <c r="AB86" s="361"/>
+      <c r="AC86" s="363"/>
+      <c r="AD86" s="364"/>
+      <c r="AE86" s="364"/>
     </row>
     <row r="87" spans="1:31" ht="15.75" thickBot="1">
       <c r="A87" s="13"/>
-      <c r="N87" s="357" t="s">
+      <c r="N87" s="365" t="s">
         <v>28</v>
       </c>
-      <c r="O87" s="358"/>
-      <c r="P87" s="358"/>
-      <c r="Q87" s="358"/>
-      <c r="R87" s="358"/>
-      <c r="S87" s="358"/>
-      <c r="T87" s="358"/>
-      <c r="U87" s="358"/>
-      <c r="V87" s="358"/>
-      <c r="W87" s="359"/>
-      <c r="X87" s="344">
+      <c r="O87" s="366"/>
+      <c r="P87" s="366"/>
+      <c r="Q87" s="366"/>
+      <c r="R87" s="366"/>
+      <c r="S87" s="366"/>
+      <c r="T87" s="366"/>
+      <c r="U87" s="366"/>
+      <c r="V87" s="366"/>
+      <c r="W87" s="367"/>
+      <c r="X87" s="352">
         <f t="shared" ref="X87:AC87" si="11">COUNTIF(X13:X77,"&gt;=" &amp;X85)</f>
         <v>54</v>
       </c>
-      <c r="Y87" s="346">
+      <c r="Y87" s="354">
         <f t="shared" si="11"/>
         <v>52</v>
       </c>
-      <c r="Z87" s="348">
+      <c r="Z87" s="356">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AA87" s="350">
+      <c r="AA87" s="358">
         <f t="shared" si="11"/>
         <v>58</v>
       </c>
-      <c r="AB87" s="352">
+      <c r="AB87" s="360">
         <f t="shared" si="11"/>
         <v>37</v>
       </c>
-      <c r="AC87" s="354">
+      <c r="AC87" s="362">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD87" s="356"/>
-      <c r="AE87" s="356"/>
+      <c r="AD87" s="364"/>
+      <c r="AE87" s="364"/>
     </row>
     <row r="88" spans="1:31" ht="9" customHeight="1" thickBot="1">
-      <c r="N88" s="360"/>
-      <c r="O88" s="361"/>
-      <c r="P88" s="361"/>
-      <c r="Q88" s="361"/>
-      <c r="R88" s="361"/>
-      <c r="S88" s="361"/>
-      <c r="T88" s="361"/>
-      <c r="U88" s="361"/>
-      <c r="V88" s="361"/>
-      <c r="W88" s="362"/>
-      <c r="X88" s="345"/>
-      <c r="Y88" s="347"/>
-      <c r="Z88" s="349"/>
-      <c r="AA88" s="351"/>
-      <c r="AB88" s="353"/>
-      <c r="AC88" s="355"/>
-      <c r="AD88" s="356"/>
-      <c r="AE88" s="356"/>
+      <c r="N88" s="368"/>
+      <c r="O88" s="369"/>
+      <c r="P88" s="369"/>
+      <c r="Q88" s="369"/>
+      <c r="R88" s="369"/>
+      <c r="S88" s="369"/>
+      <c r="T88" s="369"/>
+      <c r="U88" s="369"/>
+      <c r="V88" s="369"/>
+      <c r="W88" s="370"/>
+      <c r="X88" s="353"/>
+      <c r="Y88" s="355"/>
+      <c r="Z88" s="357"/>
+      <c r="AA88" s="359"/>
+      <c r="AB88" s="361"/>
+      <c r="AC88" s="363"/>
+      <c r="AD88" s="364"/>
+      <c r="AE88" s="364"/>
     </row>
     <row r="91" spans="1:31" ht="15.75" thickBot="1"/>
     <row r="92" spans="1:31" ht="43.5" customHeight="1" thickBot="1">
-      <c r="B92" s="335" t="s">
+      <c r="B92" s="343" t="s">
         <v>34</v>
       </c>
-      <c r="C92" s="336"/>
-      <c r="D92" s="336"/>
-      <c r="E92" s="337"/>
-      <c r="F92" s="323" t="s">
+      <c r="C92" s="344"/>
+      <c r="D92" s="344"/>
+      <c r="E92" s="345"/>
+      <c r="F92" s="331" t="s">
         <v>38</v>
       </c>
-      <c r="G92" s="323"/>
-      <c r="H92" s="324"/>
+      <c r="G92" s="331"/>
+      <c r="H92" s="332"/>
       <c r="I92" s="262" t="s">
         <v>39</v>
       </c>
       <c r="J92" s="263"/>
     </row>
     <row r="93" spans="1:31">
-      <c r="B93" s="326" t="s">
+      <c r="B93" s="334" t="s">
         <v>35</v>
       </c>
-      <c r="C93" s="329" t="s">
+      <c r="C93" s="337" t="s">
         <v>44</v>
       </c>
-      <c r="D93" s="329"/>
-      <c r="E93" s="330"/>
-      <c r="F93" s="338">
+      <c r="D93" s="337"/>
+      <c r="E93" s="338"/>
+      <c r="F93" s="346">
         <v>66</v>
       </c>
-      <c r="G93" s="329"/>
+      <c r="G93" s="337"/>
       <c r="H93" s="18">
         <f>0.2*F93</f>
         <v>13.200000000000001</v>
@@ -11428,14 +11428,14 @@
       <c r="J93" s="265"/>
     </row>
     <row r="94" spans="1:31">
-      <c r="B94" s="327"/>
-      <c r="C94" s="331" t="s">
+      <c r="B94" s="335"/>
+      <c r="C94" s="339" t="s">
         <v>36</v>
       </c>
-      <c r="D94" s="331"/>
-      <c r="E94" s="332"/>
-      <c r="F94" s="339"/>
-      <c r="G94" s="331"/>
+      <c r="D94" s="339"/>
+      <c r="E94" s="340"/>
+      <c r="F94" s="347"/>
+      <c r="G94" s="339"/>
       <c r="H94" s="19">
         <f>0.4*F93</f>
         <v>26.400000000000002</v>
@@ -11446,14 +11446,14 @@
       <c r="J94" s="267"/>
     </row>
     <row r="95" spans="1:31" ht="15.75" thickBot="1">
-      <c r="B95" s="328"/>
-      <c r="C95" s="333" t="s">
+      <c r="B95" s="336"/>
+      <c r="C95" s="341" t="s">
         <v>37</v>
       </c>
-      <c r="D95" s="333"/>
-      <c r="E95" s="334"/>
-      <c r="F95" s="340"/>
-      <c r="G95" s="333"/>
+      <c r="D95" s="341"/>
+      <c r="E95" s="342"/>
+      <c r="F95" s="348"/>
+      <c r="G95" s="341"/>
       <c r="H95" s="20">
         <f>0.6*F93</f>
         <v>39.6</v>
@@ -11467,14 +11467,14 @@
       </c>
     </row>
     <row r="96" spans="1:31">
-      <c r="H96" s="325"/>
-      <c r="I96" s="325"/>
-      <c r="J96" s="325"/>
+      <c r="H96" s="333"/>
+      <c r="I96" s="333"/>
+      <c r="J96" s="333"/>
     </row>
     <row r="97" spans="3:31" ht="15.75" thickBot="1">
-      <c r="H97" s="325"/>
-      <c r="I97" s="325"/>
-      <c r="J97" s="325"/>
+      <c r="H97" s="333"/>
+      <c r="I97" s="333"/>
+      <c r="J97" s="333"/>
     </row>
     <row r="98" spans="3:31" ht="24" customHeight="1">
       <c r="C98" s="23" t="s">
@@ -11625,7 +11625,7 @@
   </sheetPr>
   <dimension ref="A1:V96"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A67" zoomScale="112" zoomScaleSheetLayoutView="112" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="112" zoomScaleSheetLayoutView="112" workbookViewId="0">
       <selection activeCell="E14" sqref="E14:E79"/>
     </sheetView>
   </sheetViews>
@@ -11640,13 +11640,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="20.25">
-      <c r="B1" s="393" t="s">
+      <c r="B1" s="401" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="393"/>
-      <c r="D1" s="393"/>
-      <c r="E1" s="393"/>
-      <c r="F1" s="393"/>
+      <c r="C1" s="401"/>
+      <c r="D1" s="401"/>
+      <c r="E1" s="401"/>
+      <c r="F1" s="401"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -11822,41 +11822,41 @@
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1"/>
     <row r="9" spans="2:22" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="392" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="395" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="390" t="s">
+      <c r="B9" s="400" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="403" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="398" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="395" t="s">
+      <c r="E9" s="403" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B10" s="392"/>
-      <c r="C10" s="396"/>
-      <c r="D10" s="390"/>
-      <c r="E10" s="396"/>
+      <c r="B10" s="400"/>
+      <c r="C10" s="404"/>
+      <c r="D10" s="398"/>
+      <c r="E10" s="404"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B11" s="392"/>
-      <c r="C11" s="396"/>
-      <c r="D11" s="390"/>
-      <c r="E11" s="396"/>
+      <c r="B11" s="400"/>
+      <c r="C11" s="404"/>
+      <c r="D11" s="398"/>
+      <c r="E11" s="404"/>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B12" s="392"/>
-      <c r="C12" s="396"/>
-      <c r="D12" s="390"/>
-      <c r="E12" s="396"/>
+      <c r="B12" s="400"/>
+      <c r="C12" s="404"/>
+      <c r="D12" s="398"/>
+      <c r="E12" s="404"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B13" s="392"/>
-      <c r="C13" s="397"/>
-      <c r="D13" s="390"/>
+      <c r="B13" s="400"/>
+      <c r="C13" s="405"/>
+      <c r="D13" s="398"/>
       <c r="E13" s="186">
         <v>70</v>
       </c>
@@ -12657,7 +12657,7 @@
       <c r="D80" s="282" t="s">
         <v>57</v>
       </c>
-      <c r="E80" s="394">
+      <c r="E80" s="402">
         <f>D81*E13/100</f>
         <v>23.407999999999998</v>
       </c>
@@ -12666,7 +12666,7 @@
       <c r="D81" s="286">
         <v>33.44</v>
       </c>
-      <c r="E81" s="394"/>
+      <c r="E81" s="402"/>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="D82" s="53" t="s">
@@ -12690,30 +12690,30 @@
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="86" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A86" s="400" t="s">
+      <c r="A86" s="408" t="s">
         <v>34</v>
       </c>
-      <c r="B86" s="401"/>
-      <c r="C86" s="401"/>
-      <c r="D86" s="402"/>
-      <c r="E86" s="323" t="s">
+      <c r="B86" s="409"/>
+      <c r="C86" s="409"/>
+      <c r="D86" s="410"/>
+      <c r="E86" s="331" t="s">
         <v>38</v>
       </c>
-      <c r="F86" s="324"/>
+      <c r="F86" s="332"/>
       <c r="G86" s="46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1">
-      <c r="A87" s="403" t="s">
+      <c r="A87" s="411" t="s">
         <v>35</v>
       </c>
-      <c r="B87" s="406" t="s">
+      <c r="B87" s="414" t="s">
         <v>56</v>
       </c>
-      <c r="C87" s="406"/>
-      <c r="D87" s="407"/>
-      <c r="E87" s="408">
+      <c r="C87" s="414"/>
+      <c r="D87" s="415"/>
+      <c r="E87" s="416">
         <v>66</v>
       </c>
       <c r="F87" s="50">
@@ -12725,13 +12725,13 @@
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="404"/>
-      <c r="B88" s="331" t="s">
+      <c r="A88" s="412"/>
+      <c r="B88" s="339" t="s">
         <v>55</v>
       </c>
-      <c r="C88" s="331"/>
-      <c r="D88" s="332"/>
-      <c r="E88" s="409"/>
+      <c r="C88" s="339"/>
+      <c r="D88" s="340"/>
+      <c r="E88" s="417"/>
       <c r="F88" s="19">
         <f>0.65*$E87</f>
         <v>42.9</v>
@@ -12741,13 +12741,13 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A89" s="405"/>
-      <c r="B89" s="333" t="s">
+      <c r="A89" s="413"/>
+      <c r="B89" s="341" t="s">
         <v>54</v>
       </c>
-      <c r="C89" s="333"/>
-      <c r="D89" s="334"/>
-      <c r="E89" s="410"/>
+      <c r="C89" s="341"/>
+      <c r="D89" s="342"/>
+      <c r="E89" s="418"/>
       <c r="F89" s="51">
         <f>0.75*$E87</f>
         <v>49.5</v>
@@ -12758,10 +12758,10 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="91" spans="1:8" ht="71.25" customHeight="1">
-      <c r="A91" s="411" t="s">
+      <c r="A91" s="419" t="s">
         <v>51</v>
       </c>
-      <c r="B91" s="412"/>
+      <c r="B91" s="420"/>
       <c r="C91" s="24" t="s">
         <v>25</v>
       </c>
@@ -12782,10 +12782,10 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" thickBot="1">
-      <c r="A92" s="398" t="s">
+      <c r="A92" s="406" t="s">
         <v>52</v>
       </c>
-      <c r="B92" s="399"/>
+      <c r="B92" s="407"/>
       <c r="C92" s="27">
         <f>IF(E82&gt;=$F89,3,IF(E82&gt;=$F88,2,IF(E82&gt;=$F87,1,0)))</f>
         <v>0</v>
@@ -12861,8 +12861,8 @@
   </sheetPr>
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12959,53 +12959,53 @@
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1"/>
     <row r="9" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="392" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="395" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="430" t="s">
+      <c r="B9" s="400" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="403" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="438" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="395" t="s">
+      <c r="E9" s="403" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="431" t="s">
+      <c r="F9" s="439" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="395" t="s">
+      <c r="G9" s="403" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B10" s="392"/>
-      <c r="C10" s="396"/>
-      <c r="D10" s="430"/>
-      <c r="E10" s="396"/>
-      <c r="F10" s="432"/>
-      <c r="G10" s="396"/>
+      <c r="B10" s="400"/>
+      <c r="C10" s="404"/>
+      <c r="D10" s="438"/>
+      <c r="E10" s="404"/>
+      <c r="F10" s="440"/>
+      <c r="G10" s="404"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B11" s="392"/>
-      <c r="C11" s="396"/>
-      <c r="D11" s="430"/>
-      <c r="E11" s="396"/>
-      <c r="F11" s="432"/>
-      <c r="G11" s="396"/>
+      <c r="B11" s="400"/>
+      <c r="C11" s="404"/>
+      <c r="D11" s="438"/>
+      <c r="E11" s="404"/>
+      <c r="F11" s="440"/>
+      <c r="G11" s="404"/>
     </row>
     <row r="12" spans="2:8" ht="42" customHeight="1" thickBot="1">
-      <c r="B12" s="392"/>
-      <c r="C12" s="396"/>
-      <c r="D12" s="430"/>
-      <c r="E12" s="427"/>
-      <c r="F12" s="433"/>
-      <c r="G12" s="427"/>
+      <c r="B12" s="400"/>
+      <c r="C12" s="404"/>
+      <c r="D12" s="438"/>
+      <c r="E12" s="435"/>
+      <c r="F12" s="441"/>
+      <c r="G12" s="435"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B13" s="392"/>
-      <c r="C13" s="397"/>
-      <c r="D13" s="430"/>
+      <c r="B13" s="400"/>
+      <c r="C13" s="405"/>
+      <c r="D13" s="438"/>
       <c r="E13" s="56">
         <v>10</v>
       </c>
@@ -13032,11 +13032,9 @@
         <v>8</v>
       </c>
       <c r="F14" s="230">
-        <v>22</v>
-      </c>
-      <c r="G14" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G14" s="230"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="10">
@@ -13056,9 +13054,7 @@
       <c r="F15" s="230">
         <v>24</v>
       </c>
-      <c r="G15" s="230">
-        <v>24</v>
-      </c>
+      <c r="G15" s="230"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="10">
@@ -13073,14 +13069,12 @@
         <v>BALURE PRERANA KESHAV</v>
       </c>
       <c r="E16" s="230">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="230">
-        <v>20</v>
-      </c>
-      <c r="G16" s="230">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G16" s="230"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="10">
@@ -13100,9 +13094,7 @@
       <c r="F17" s="230">
         <v>24</v>
       </c>
-      <c r="G17" s="230">
-        <v>23</v>
-      </c>
+      <c r="G17" s="230"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="10">
@@ -13120,11 +13112,9 @@
         <v>10</v>
       </c>
       <c r="F18" s="230">
-        <v>22</v>
-      </c>
-      <c r="G18" s="230">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G18" s="230"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="10">
@@ -13144,9 +13134,7 @@
       <c r="F19" s="230">
         <v>24</v>
       </c>
-      <c r="G19" s="230">
-        <v>24</v>
-      </c>
+      <c r="G19" s="230"/>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="10">
@@ -13161,14 +13149,12 @@
         <v>BIRAJDAR SHRIDEVI UDDHAV</v>
       </c>
       <c r="E20" s="230">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="230">
         <v>22</v>
       </c>
-      <c r="G20" s="230">
-        <v>21</v>
-      </c>
+      <c r="G20" s="230"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="10">
@@ -13183,14 +13169,12 @@
         <v>BIRAJDAR SNEHAL SATISH</v>
       </c>
       <c r="E21" s="230">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="230">
         <v>24</v>
       </c>
-      <c r="G21" s="230">
-        <v>23</v>
-      </c>
+      <c r="G21" s="230"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="10">
@@ -13210,9 +13194,7 @@
       <c r="F22" s="230">
         <v>24</v>
       </c>
-      <c r="G22" s="230">
-        <v>23</v>
-      </c>
+      <c r="G22" s="230"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="10">
@@ -13227,14 +13209,12 @@
         <v>CHAFEKARANDE AKANKSHA B.</v>
       </c>
       <c r="E23" s="230">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="230">
-        <v>24</v>
-      </c>
-      <c r="G23" s="230">
         <v>23</v>
       </c>
+      <c r="G23" s="230"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="10">
@@ -13249,14 +13229,12 @@
         <v>CHANDE ANKITA RAJKUMAR</v>
       </c>
       <c r="E24" s="230">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24" s="230">
-        <v>20</v>
-      </c>
-      <c r="G24" s="230">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G24" s="230"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="10">
@@ -13271,14 +13249,12 @@
         <v>CHATAP PARVATI SHRIHARI</v>
       </c>
       <c r="E25" s="230">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="230">
-        <v>18</v>
-      </c>
-      <c r="G25" s="230">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G25" s="230"/>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="10">
@@ -13293,14 +13269,12 @@
         <v>DHOTRE SWETA SANJAY</v>
       </c>
       <c r="E26" s="230">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F26" s="230">
-        <v>22</v>
-      </c>
-      <c r="G26" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G26" s="230"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="10">
@@ -13318,11 +13292,9 @@
         <v>6</v>
       </c>
       <c r="F27" s="230">
-        <v>22</v>
-      </c>
-      <c r="G27" s="230">
         <v>21</v>
       </c>
+      <c r="G27" s="230"/>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="10">
@@ -13337,14 +13309,12 @@
         <v>DIGGIKAR BHAVANA VIJAY</v>
       </c>
       <c r="E28" s="230">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F28" s="230">
-        <v>18</v>
-      </c>
-      <c r="G28" s="230">
-        <v>15</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G28" s="230"/>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="10">
@@ -13362,11 +13332,9 @@
         <v>5</v>
       </c>
       <c r="F29" s="230">
-        <v>16</v>
-      </c>
-      <c r="G29" s="230">
-        <v>14</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G29" s="230"/>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="10">
@@ -13380,15 +13348,9 @@
         <f>'CO_Attainment for Unit Tests'!C29</f>
         <v>HANGE VAJRASHRI MADHAV</v>
       </c>
-      <c r="E30" s="230">
-        <v>5</v>
-      </c>
-      <c r="F30" s="230">
-        <v>15</v>
-      </c>
-      <c r="G30" s="230">
-        <v>12</v>
-      </c>
+      <c r="E30" s="230"/>
+      <c r="F30" s="230"/>
+      <c r="G30" s="230"/>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="10">
@@ -13406,11 +13368,9 @@
         <v>10</v>
       </c>
       <c r="F31" s="230">
-        <v>22</v>
-      </c>
-      <c r="G31" s="230">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G31" s="230"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="10">
@@ -13430,9 +13390,7 @@
       <c r="F32" s="230">
         <v>24</v>
       </c>
-      <c r="G32" s="230">
-        <v>22</v>
-      </c>
+      <c r="G32" s="230"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="10">
@@ -13447,14 +13405,12 @@
         <v>JADHAV SIMRAN GOKUL</v>
       </c>
       <c r="E33" s="230">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F33" s="230">
-        <v>19</v>
-      </c>
-      <c r="G33" s="230">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G33" s="230"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="10">
@@ -13469,14 +13425,12 @@
         <v>JOSHI SANJIVANI SANJAY</v>
       </c>
       <c r="E34" s="230">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F34" s="230">
-        <v>16</v>
-      </c>
-      <c r="G34" s="230">
-        <v>16</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G34" s="230"/>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="10">
@@ -13491,14 +13445,12 @@
         <v>KADAM PUNAM SHRIHARI</v>
       </c>
       <c r="E35" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" s="230">
         <v>24</v>
       </c>
-      <c r="G35" s="230">
-        <v>22</v>
-      </c>
+      <c r="G35" s="230"/>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="10">
@@ -13513,14 +13465,12 @@
         <v>KAMBLE PRANALI JITENDRA</v>
       </c>
       <c r="E36" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F36" s="230">
-        <v>20</v>
-      </c>
-      <c r="G36" s="230">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G36" s="230"/>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="10">
@@ -13535,14 +13485,12 @@
         <v>KAMBLE PRIYA VILAS</v>
       </c>
       <c r="E37" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F37" s="230">
-        <v>20</v>
-      </c>
-      <c r="G37" s="230">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G37" s="230"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="10">
@@ -13562,9 +13510,7 @@
       <c r="F38" s="230">
         <v>24</v>
       </c>
-      <c r="G38" s="230">
-        <v>24</v>
-      </c>
+      <c r="G38" s="230"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="10">
@@ -13582,11 +13528,9 @@
         <v>9</v>
       </c>
       <c r="F39" s="230">
-        <v>21</v>
-      </c>
-      <c r="G39" s="230">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G39" s="230"/>
     </row>
     <row r="40" spans="2:7">
       <c r="B40" s="10">
@@ -13606,9 +13550,7 @@
       <c r="F40" s="230">
         <v>24</v>
       </c>
-      <c r="G40" s="230">
-        <v>24</v>
-      </c>
+      <c r="G40" s="230"/>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="10">
@@ -13626,11 +13568,9 @@
         <v>10</v>
       </c>
       <c r="F41" s="230">
-        <v>24</v>
-      </c>
-      <c r="G41" s="230">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G41" s="230"/>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="10">
@@ -13645,14 +13585,12 @@
         <v>MANE SAKSHI SANTOSH</v>
       </c>
       <c r="E42" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F42" s="230">
-        <v>19</v>
-      </c>
-      <c r="G42" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G42" s="230"/>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="10">
@@ -13670,11 +13608,9 @@
         <v>8</v>
       </c>
       <c r="F43" s="230">
-        <v>22</v>
-      </c>
-      <c r="G43" s="230">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G43" s="230"/>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="10">
@@ -13689,14 +13625,12 @@
         <v>MORE SHITAL BHARAT</v>
       </c>
       <c r="E44" s="230">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="230">
-        <v>20</v>
-      </c>
-      <c r="G44" s="230">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G44" s="230"/>
     </row>
     <row r="45" spans="2:7">
       <c r="B45" s="10">
@@ -13711,14 +13645,12 @@
         <v>MORE SHWETA SANJAY</v>
       </c>
       <c r="E45" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F45" s="230">
-        <v>22</v>
-      </c>
-      <c r="G45" s="230">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G45" s="230"/>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" s="10">
@@ -13733,14 +13665,12 @@
         <v>NADGIRE SHIVANI SANTOSH</v>
       </c>
       <c r="E46" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F46" s="230">
-        <v>22</v>
-      </c>
-      <c r="G46" s="230">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G46" s="230"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="10">
@@ -13755,14 +13685,12 @@
         <v xml:space="preserve">NAGWANSHI PRERNA N </v>
       </c>
       <c r="E47" s="230">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F47" s="230">
-        <v>22</v>
-      </c>
-      <c r="G47" s="230">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G47" s="230"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="10">
@@ -13777,14 +13705,12 @@
         <v>PATE ASHVINI ARVIND</v>
       </c>
       <c r="E48" s="230">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F48" s="230">
-        <v>22</v>
-      </c>
-      <c r="G48" s="230">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G48" s="230"/>
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="10">
@@ -13799,14 +13725,12 @@
         <v>PATIL ADITI SANJAY</v>
       </c>
       <c r="E49" s="230">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F49" s="230">
-        <v>19</v>
-      </c>
-      <c r="G49" s="230">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G49" s="230"/>
     </row>
     <row r="50" spans="2:7">
       <c r="B50" s="10">
@@ -13824,11 +13748,9 @@
         <v>5</v>
       </c>
       <c r="F50" s="230">
-        <v>16</v>
-      </c>
-      <c r="G50" s="230">
-        <v>15</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G50" s="230"/>
     </row>
     <row r="51" spans="2:7">
       <c r="B51" s="10">
@@ -13848,9 +13770,7 @@
       <c r="F51" s="230">
         <v>24</v>
       </c>
-      <c r="G51" s="230">
-        <v>24</v>
-      </c>
+      <c r="G51" s="230"/>
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="10">
@@ -13865,14 +13785,12 @@
         <v>PATIL VAISHNAVI RAYABA</v>
       </c>
       <c r="E52" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F52" s="230">
-        <v>19</v>
-      </c>
-      <c r="G52" s="230">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G52" s="230"/>
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="10">
@@ -13887,14 +13805,12 @@
         <v>PAWAR SAKSHI SHARAD</v>
       </c>
       <c r="E53" s="230">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F53" s="230">
-        <v>15</v>
-      </c>
-      <c r="G53" s="230">
-        <v>17</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G53" s="230"/>
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="10">
@@ -13909,14 +13825,12 @@
         <v xml:space="preserve">POTDAR VAISHNAVI S </v>
       </c>
       <c r="E54" s="230">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F54" s="230">
-        <v>21</v>
-      </c>
-      <c r="G54" s="230">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G54" s="230"/>
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="10">
@@ -13934,11 +13848,9 @@
         <v>8</v>
       </c>
       <c r="F55" s="230">
-        <v>20</v>
-      </c>
-      <c r="G55" s="230">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G55" s="230"/>
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="10">
@@ -13953,14 +13865,12 @@
         <v xml:space="preserve">RAJURE VAISHNAVI V </v>
       </c>
       <c r="E56" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F56" s="230">
         <v>21</v>
       </c>
-      <c r="G56" s="230">
-        <v>22</v>
-      </c>
+      <c r="G56" s="230"/>
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="10">
@@ -13975,14 +13885,12 @@
         <v xml:space="preserve">SABLE SHITAL S </v>
       </c>
       <c r="E57" s="230">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F57" s="230">
-        <v>19</v>
-      </c>
-      <c r="G57" s="230">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G57" s="230"/>
     </row>
     <row r="58" spans="2:7">
       <c r="B58" s="10">
@@ -13997,14 +13905,12 @@
         <v xml:space="preserve">SALUNKE APEKSHA N </v>
       </c>
       <c r="E58" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F58" s="230">
         <v>22</v>
       </c>
-      <c r="G58" s="230">
-        <v>21</v>
-      </c>
+      <c r="G58" s="230"/>
     </row>
     <row r="59" spans="2:7">
       <c r="B59" s="10">
@@ -14019,14 +13925,12 @@
         <v xml:space="preserve">SAVANT VAISHNAVI B </v>
       </c>
       <c r="E59" s="230">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F59" s="230">
-        <v>22</v>
-      </c>
-      <c r="G59" s="230">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G59" s="230"/>
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="10">
@@ -14041,14 +13945,12 @@
         <v xml:space="preserve">SAWANT SNEHAL R </v>
       </c>
       <c r="E60" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F60" s="230">
-        <v>22</v>
-      </c>
-      <c r="G60" s="230">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G60" s="230"/>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="10">
@@ -14063,14 +13965,12 @@
         <v xml:space="preserve">SHAIKH SANIYA T </v>
       </c>
       <c r="E61" s="230">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F61" s="230">
-        <v>23</v>
-      </c>
-      <c r="G61" s="230">
         <v>24</v>
       </c>
+      <c r="G61" s="230"/>
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="10">
@@ -14085,14 +13985,12 @@
         <v xml:space="preserve">SHINDE ADITI K </v>
       </c>
       <c r="E62" s="230">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" s="230">
-        <v>23</v>
-      </c>
-      <c r="G62" s="230">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G62" s="230"/>
     </row>
     <row r="63" spans="2:7">
       <c r="B63" s="10">
@@ -14107,14 +14005,12 @@
         <v xml:space="preserve">SHINDE ROHINI A </v>
       </c>
       <c r="E63" s="230">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" s="230">
-        <v>22</v>
-      </c>
-      <c r="G63" s="230">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G63" s="230"/>
     </row>
     <row r="64" spans="2:7">
       <c r="B64" s="10">
@@ -14129,14 +14025,12 @@
         <v xml:space="preserve">SURYAWANSHI PRANJALI S </v>
       </c>
       <c r="E64" s="230">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F64" s="230">
-        <v>22</v>
-      </c>
-      <c r="G64" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G64" s="230"/>
     </row>
     <row r="65" spans="2:7">
       <c r="B65" s="10">
@@ -14151,14 +14045,12 @@
         <v xml:space="preserve">TADLAPURE NEHA H </v>
       </c>
       <c r="E65" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F65" s="230">
-        <v>23</v>
-      </c>
-      <c r="G65" s="230">
         <v>24</v>
       </c>
+      <c r="G65" s="230"/>
     </row>
     <row r="66" spans="2:7">
       <c r="B66" s="10">
@@ -14173,14 +14065,12 @@
         <v xml:space="preserve">TAKALE VAISHNAVI B </v>
       </c>
       <c r="E66" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F66" s="230">
-        <v>21</v>
-      </c>
-      <c r="G66" s="230">
         <v>23</v>
       </c>
+      <c r="G66" s="230"/>
     </row>
     <row r="67" spans="2:7">
       <c r="B67" s="10">
@@ -14195,14 +14085,12 @@
         <v>TARE ANKITA ANIL</v>
       </c>
       <c r="E67" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F67" s="230">
         <v>23</v>
       </c>
-      <c r="G67" s="230">
-        <v>22</v>
-      </c>
+      <c r="G67" s="230"/>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" s="10">
@@ -14217,14 +14105,12 @@
         <v>TONDARE SHRADDHA D.</v>
       </c>
       <c r="E68" s="230">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F68" s="230">
-        <v>21</v>
-      </c>
-      <c r="G68" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G68" s="230"/>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" s="10">
@@ -14239,14 +14125,12 @@
         <v xml:space="preserve">WAGHMARE RUKMIN S </v>
       </c>
       <c r="E69" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F69" s="230">
-        <v>22</v>
-      </c>
-      <c r="G69" s="230">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G69" s="230"/>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" s="10">
@@ -14264,11 +14148,9 @@
         <v>8</v>
       </c>
       <c r="F70" s="230">
-        <v>22</v>
-      </c>
-      <c r="G70" s="230">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G70" s="230"/>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" s="10">
@@ -14288,9 +14170,7 @@
       <c r="F71" s="230">
         <v>24</v>
       </c>
-      <c r="G71" s="230">
-        <v>23</v>
-      </c>
+      <c r="G71" s="230"/>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" s="10">
@@ -14305,14 +14185,12 @@
         <v xml:space="preserve">MALBHAGE ASHVINI G </v>
       </c>
       <c r="E72" s="230">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F72" s="230">
         <v>22</v>
       </c>
-      <c r="G72" s="230">
-        <v>21</v>
-      </c>
+      <c r="G72" s="230"/>
     </row>
     <row r="73" spans="2:7">
       <c r="B73" s="10">
@@ -14327,14 +14205,12 @@
         <v xml:space="preserve">Vanjary Prinka </v>
       </c>
       <c r="E73" s="230">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F73" s="230">
-        <v>14</v>
-      </c>
-      <c r="G73" s="230">
-        <v>16</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G73" s="230"/>
     </row>
     <row r="74" spans="2:7">
       <c r="B74" s="10">
@@ -14348,15 +14224,9 @@
         <f>'CO_Attainment for Unit Tests'!C73</f>
         <v>Panchal Punam Vishnu</v>
       </c>
-      <c r="E74" s="230">
-        <v>9</v>
-      </c>
-      <c r="F74" s="230">
-        <v>19</v>
-      </c>
-      <c r="G74" s="230">
-        <v>18</v>
-      </c>
+      <c r="E74" s="230"/>
+      <c r="F74" s="230"/>
+      <c r="G74" s="230"/>
     </row>
     <row r="75" spans="2:7">
       <c r="B75" s="10">
@@ -14374,11 +14244,9 @@
         <v>9</v>
       </c>
       <c r="F75" s="230">
-        <v>16</v>
-      </c>
-      <c r="G75" s="230">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G75" s="230"/>
     </row>
     <row r="76" spans="2:7">
       <c r="B76" s="10">
@@ -14393,14 +14261,12 @@
         <v>Deshpande Nikita S</v>
       </c>
       <c r="E76" s="230">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F76" s="230">
-        <v>18</v>
-      </c>
-      <c r="G76" s="230">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G76" s="230"/>
     </row>
     <row r="77" spans="2:7">
       <c r="B77" s="10">
@@ -14415,14 +14281,12 @@
         <v>Kharte Sneha Jotiram</v>
       </c>
       <c r="E77" s="230">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F77" s="230">
-        <v>20</v>
-      </c>
-      <c r="G77" s="230">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G77" s="230"/>
     </row>
     <row r="78" spans="2:7">
       <c r="B78" s="10">
@@ -14437,14 +14301,12 @@
         <v>Fulari  Nikita Sangappa</v>
       </c>
       <c r="E78" s="230">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F78" s="230">
-        <v>18</v>
-      </c>
-      <c r="G78" s="230">
-        <v>18</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G78" s="230"/>
     </row>
     <row r="79" spans="2:7" ht="14.25" customHeight="1">
       <c r="B79" s="138">
@@ -14458,15 +14320,9 @@
         <f>'CO_Attainment for Unit Tests'!C78</f>
         <v>Gaikwad Mohini Y.</v>
       </c>
-      <c r="E79" s="230">
-        <v>8</v>
-      </c>
-      <c r="F79" s="230">
-        <v>18</v>
-      </c>
-      <c r="G79" s="230">
-        <v>17</v>
-      </c>
+      <c r="E79" s="230"/>
+      <c r="F79" s="230"/>
+      <c r="G79" s="230"/>
     </row>
     <row r="80" spans="2:7" ht="15.75" thickBot="1">
       <c r="B80" s="12"/>
@@ -14477,27 +14333,27 @@
       <c r="G80" s="12"/>
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1">
-      <c r="D81" s="428" t="s">
+      <c r="D81" s="436" t="s">
         <v>64</v>
       </c>
-      <c r="E81" s="428">
+      <c r="E81" s="436">
         <f>ROUNDUP(0.6*E13,1)</f>
         <v>6</v>
       </c>
-      <c r="F81" s="428">
+      <c r="F81" s="436">
         <f>ROUNDUP(0.6*F13,1)</f>
         <v>15</v>
       </c>
-      <c r="G81" s="428">
+      <c r="G81" s="436">
         <f>ROUNDUP(0.6*G13,1)</f>
         <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D82" s="429"/>
-      <c r="E82" s="429"/>
-      <c r="F82" s="429"/>
-      <c r="G82" s="429"/>
+      <c r="D82" s="437"/>
+      <c r="E82" s="437"/>
+      <c r="F82" s="437"/>
+      <c r="G82" s="437"/>
     </row>
     <row r="83" spans="1:8" ht="16.5" thickBot="1">
       <c r="D83" s="53" t="s">
@@ -14505,41 +14361,41 @@
       </c>
       <c r="E83" s="54">
         <f>COUNTIF(E14:E80,"&gt;=" &amp;E81)</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F83" s="54">
         <f>COUNTIF(F14:F80,"&gt;=" &amp;F81)</f>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G83" s="54">
         <f>COUNTIF(G14:G80,"&gt;=" &amp;G81)</f>
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="86" spans="1:8" ht="46.5" customHeight="1" thickBot="1">
-      <c r="B86" s="400" t="s">
+      <c r="B86" s="408" t="s">
         <v>63</v>
       </c>
-      <c r="C86" s="401"/>
-      <c r="D86" s="402"/>
-      <c r="E86" s="323" t="s">
+      <c r="C86" s="409"/>
+      <c r="D86" s="410"/>
+      <c r="E86" s="331" t="s">
         <v>38</v>
       </c>
-      <c r="F86" s="324"/>
+      <c r="F86" s="332"/>
       <c r="G86" s="46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="B87" s="403" t="s">
+      <c r="B87" s="411" t="s">
         <v>35</v>
       </c>
-      <c r="C87" s="421" t="s">
+      <c r="C87" s="429" t="s">
         <v>37</v>
       </c>
-      <c r="D87" s="422"/>
-      <c r="E87" s="408">
+      <c r="D87" s="430"/>
+      <c r="E87" s="416">
         <v>66</v>
       </c>
       <c r="F87" s="50">
@@ -14551,12 +14407,12 @@
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="B88" s="404"/>
-      <c r="C88" s="423" t="s">
+      <c r="B88" s="412"/>
+      <c r="C88" s="431" t="s">
         <v>66</v>
       </c>
-      <c r="D88" s="424"/>
-      <c r="E88" s="409"/>
+      <c r="D88" s="432"/>
+      <c r="E88" s="417"/>
       <c r="F88" s="19">
         <f>0.7*$E87</f>
         <v>46.199999999999996</v>
@@ -14566,12 +14422,12 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" thickBot="1">
-      <c r="B89" s="405"/>
-      <c r="C89" s="425" t="s">
+      <c r="B89" s="413"/>
+      <c r="C89" s="433" t="s">
         <v>65</v>
       </c>
-      <c r="D89" s="426"/>
-      <c r="E89" s="410"/>
+      <c r="D89" s="434"/>
+      <c r="E89" s="418"/>
       <c r="F89" s="51">
         <f>0.8*$E87</f>
         <v>52.800000000000004</v>
@@ -14582,10 +14438,10 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="91" spans="1:8" ht="33" customHeight="1" thickBot="1">
-      <c r="A91" s="419" t="s">
+      <c r="A91" s="427" t="s">
         <v>67</v>
       </c>
-      <c r="B91" s="420"/>
+      <c r="B91" s="428"/>
       <c r="C91" s="57" t="s">
         <v>25</v>
       </c>
@@ -14606,10 +14462,10 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A92" s="415" t="s">
+      <c r="A92" s="423" t="s">
         <v>68</v>
       </c>
-      <c r="B92" s="416"/>
+      <c r="B92" s="424"/>
       <c r="C92" s="59">
         <f>IF(E83&gt;=$F89,3,IF(E83&gt;=$F88,2,IF(E83&gt;=$F87,1,0)))</f>
         <v>3</v>
@@ -14636,10 +14492,10 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A93" s="413" t="s">
+      <c r="A93" s="421" t="s">
         <v>69</v>
       </c>
-      <c r="B93" s="414"/>
+      <c r="B93" s="422"/>
       <c r="C93" s="60">
         <f>IF(F83&gt;=$F89,3,IF(F83&gt;=$F88,2,IF(F83&gt;=$F87,1,0)))</f>
         <v>3</v>
@@ -14666,33 +14522,33 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A94" s="417" t="s">
+      <c r="A94" s="425" t="s">
         <v>70</v>
       </c>
-      <c r="B94" s="418"/>
+      <c r="B94" s="426"/>
       <c r="C94" s="27">
         <f>IF(G83&gt;=$F89,3,IF(G83&gt;=$F88,2,IF(G83&gt;=$F87,1,0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D94" s="27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E94" s="27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F94" s="27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G94" s="27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H94" s="63">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -14762,7 +14618,7 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A44" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
@@ -14852,41 +14708,41 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B10" s="392" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="395" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="430" t="s">
+      <c r="B10" s="400" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="403" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="438" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="395" t="s">
+      <c r="E10" s="403" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B11" s="392"/>
-      <c r="C11" s="396"/>
-      <c r="D11" s="430"/>
-      <c r="E11" s="434"/>
+      <c r="B11" s="400"/>
+      <c r="C11" s="404"/>
+      <c r="D11" s="438"/>
+      <c r="E11" s="442"/>
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B12" s="392"/>
-      <c r="C12" s="396"/>
-      <c r="D12" s="430"/>
-      <c r="E12" s="434"/>
+      <c r="B12" s="400"/>
+      <c r="C12" s="404"/>
+      <c r="D12" s="438"/>
+      <c r="E12" s="442"/>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B13" s="392"/>
-      <c r="C13" s="396"/>
-      <c r="D13" s="430"/>
-      <c r="E13" s="435"/>
+      <c r="B13" s="400"/>
+      <c r="C13" s="404"/>
+      <c r="D13" s="438"/>
+      <c r="E13" s="443"/>
     </row>
     <row r="14" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B14" s="392"/>
-      <c r="C14" s="397"/>
-      <c r="D14" s="430"/>
+      <c r="B14" s="400"/>
+      <c r="C14" s="405"/>
+      <c r="D14" s="438"/>
       <c r="E14" s="70">
         <v>5</v>
       </c>
@@ -15869,57 +15725,57 @@
     </row>
     <row r="85" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="86" spans="1:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="A86" s="400" t="s">
+      <c r="A86" s="408" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="401"/>
-      <c r="C86" s="401"/>
-      <c r="D86" s="402"/>
+      <c r="B86" s="409"/>
+      <c r="C86" s="409"/>
+      <c r="D86" s="410"/>
       <c r="E86" s="46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A87" s="403" t="s">
+      <c r="A87" s="411" t="s">
         <v>35</v>
       </c>
-      <c r="B87" s="421" t="s">
+      <c r="B87" s="429" t="s">
         <v>158</v>
       </c>
-      <c r="C87" s="438"/>
-      <c r="D87" s="439"/>
+      <c r="C87" s="446"/>
+      <c r="D87" s="447"/>
       <c r="E87" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="404"/>
-      <c r="B88" s="423" t="s">
+      <c r="A88" s="412"/>
+      <c r="B88" s="431" t="s">
         <v>159</v>
       </c>
-      <c r="C88" s="437"/>
-      <c r="D88" s="424"/>
+      <c r="C88" s="445"/>
+      <c r="D88" s="432"/>
       <c r="E88" s="48">
         <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A89" s="405"/>
-      <c r="B89" s="425" t="s">
+      <c r="A89" s="413"/>
+      <c r="B89" s="433" t="s">
         <v>160</v>
       </c>
-      <c r="C89" s="436"/>
-      <c r="D89" s="426"/>
+      <c r="C89" s="444"/>
+      <c r="D89" s="434"/>
       <c r="E89" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="91" spans="1:7" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A91" s="419" t="s">
+      <c r="A91" s="427" t="s">
         <v>67</v>
       </c>
-      <c r="B91" s="420"/>
+      <c r="B91" s="428"/>
       <c r="C91" s="57" t="s">
         <v>25</v>
       </c>
@@ -15937,10 +15793,10 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="30" customHeight="1">
-      <c r="A92" s="411" t="s">
+      <c r="A92" s="419" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="412"/>
+      <c r="B92" s="420"/>
       <c r="C92" s="59">
         <f>IF(E82&gt;=80,3,IF(E82&gt;65,2,IF(E82&gt;=40,1,0)))</f>
         <v>3</v>
@@ -16056,34 +15912,34 @@
       <c r="P5" s="29"/>
     </row>
     <row r="6" spans="2:16" ht="16.5" thickBot="1">
-      <c r="B6" s="448" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="451" t="s">
+      <c r="B6" s="456" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="459" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="452"/>
-      <c r="E6" s="440" t="s">
+      <c r="D6" s="460"/>
+      <c r="E6" s="448" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="457"/>
-      <c r="G6" s="457"/>
-      <c r="H6" s="457"/>
-      <c r="I6" s="457"/>
-      <c r="J6" s="457"/>
-      <c r="K6" s="457"/>
-      <c r="L6" s="457"/>
-      <c r="M6" s="457"/>
-      <c r="N6" s="441"/>
-      <c r="O6" s="440" t="s">
+      <c r="F6" s="465"/>
+      <c r="G6" s="465"/>
+      <c r="H6" s="465"/>
+      <c r="I6" s="465"/>
+      <c r="J6" s="465"/>
+      <c r="K6" s="465"/>
+      <c r="L6" s="465"/>
+      <c r="M6" s="465"/>
+      <c r="N6" s="449"/>
+      <c r="O6" s="448" t="s">
         <v>97</v>
       </c>
-      <c r="P6" s="441"/>
+      <c r="P6" s="449"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B7" s="449"/>
-      <c r="C7" s="453"/>
-      <c r="D7" s="454"/>
+      <c r="B7" s="457"/>
+      <c r="C7" s="461"/>
+      <c r="D7" s="462"/>
       <c r="E7" s="95" t="s">
         <v>98</v>
       </c>
@@ -16122,9 +15978,9 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="68.25" thickBot="1">
-      <c r="B8" s="450"/>
-      <c r="C8" s="455"/>
-      <c r="D8" s="456"/>
+      <c r="B8" s="458"/>
+      <c r="C8" s="463"/>
+      <c r="D8" s="464"/>
       <c r="E8" s="96" t="s">
         <v>110</v>
       </c>
@@ -16445,11 +16301,11 @@
       </c>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B15" s="445" t="s">
+      <c r="B15" s="453" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="446"/>
-      <c r="D15" s="447"/>
+      <c r="C15" s="454"/>
+      <c r="D15" s="455"/>
       <c r="E15" s="100">
         <f t="shared" ref="E15:G15" si="0">ROUNDUP(AVERAGE(E9:E14),2)</f>
         <v>3</v>
@@ -16500,11 +16356,11 @@
       </c>
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B16" s="442" t="s">
+      <c r="B16" s="450" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="443"/>
-      <c r="D16" s="444"/>
+      <c r="C16" s="451"/>
+      <c r="D16" s="452"/>
       <c r="E16" s="106">
         <f>ROUNDUP((E15*2.66)/3,2)</f>
         <v>2.66</v>
@@ -16555,11 +16411,11 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B17" s="442" t="s">
+      <c r="B17" s="450" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="443"/>
-      <c r="D17" s="444"/>
+      <c r="C17" s="451"/>
+      <c r="D17" s="452"/>
       <c r="E17" s="106">
         <f>ROUNDUP((E16/3)*100,2)</f>
         <v>88.67</v>
@@ -16697,49 +16553,49 @@
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="8" spans="2:10" ht="21.75" thickBot="1">
-      <c r="C8" s="460" t="s">
+      <c r="C8" s="468" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="461"/>
-      <c r="E8" s="461"/>
-      <c r="F8" s="461"/>
-      <c r="G8" s="461"/>
-      <c r="H8" s="461"/>
-      <c r="I8" s="461"/>
-      <c r="J8" s="462"/>
+      <c r="D8" s="469"/>
+      <c r="E8" s="469"/>
+      <c r="F8" s="469"/>
+      <c r="G8" s="469"/>
+      <c r="H8" s="469"/>
+      <c r="I8" s="469"/>
+      <c r="J8" s="470"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1">
-      <c r="C9" s="463" t="s">
+      <c r="C9" s="471" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="464"/>
-      <c r="E9" s="464"/>
-      <c r="F9" s="464"/>
-      <c r="G9" s="464"/>
-      <c r="H9" s="465"/>
-      <c r="I9" s="466" t="s">
+      <c r="D9" s="472"/>
+      <c r="E9" s="472"/>
+      <c r="F9" s="472"/>
+      <c r="G9" s="472"/>
+      <c r="H9" s="473"/>
+      <c r="I9" s="474" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="467"/>
+      <c r="J9" s="475"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1">
-      <c r="C10" s="470" t="s">
+      <c r="C10" s="478" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="472" t="s">
+      <c r="D10" s="480" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="473"/>
-      <c r="F10" s="473"/>
-      <c r="G10" s="474"/>
+      <c r="E10" s="481"/>
+      <c r="F10" s="481"/>
+      <c r="G10" s="482"/>
       <c r="H10" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="468"/>
-      <c r="J10" s="469"/>
+      <c r="I10" s="476"/>
+      <c r="J10" s="477"/>
     </row>
     <row r="11" spans="2:10" ht="45.75" customHeight="1" thickBot="1">
-      <c r="C11" s="471"/>
+      <c r="C11" s="479"/>
       <c r="D11" s="80" t="s">
         <v>77</v>
       </c>
@@ -16755,10 +16611,10 @@
       <c r="H11" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="475" t="s">
+      <c r="I11" s="483" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="476"/>
+      <c r="J11" s="484"/>
     </row>
     <row r="12" spans="2:10">
       <c r="C12" s="86" t="s">
@@ -16778,17 +16634,17 @@
       </c>
       <c r="G12" s="74">
         <f>'CO_attain_MicroP_PR-TW_ESE'!C94</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12" s="75">
         <f>'CO_attainment for ESEBoard Exam'!C92</f>
         <v>0</v>
       </c>
-      <c r="I12" s="477">
+      <c r="I12" s="485">
         <f>'CO_attainment for Indirect'!C92</f>
         <v>3</v>
       </c>
-      <c r="J12" s="478"/>
+      <c r="J12" s="486"/>
     </row>
     <row r="13" spans="2:10">
       <c r="C13" s="87" t="s">
@@ -16808,17 +16664,17 @@
       </c>
       <c r="G13" s="76">
         <f>$G12</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H13" s="77">
         <f>$H12</f>
         <v>0</v>
       </c>
-      <c r="I13" s="458">
+      <c r="I13" s="466">
         <f>$I12</f>
         <v>3</v>
       </c>
-      <c r="J13" s="459"/>
+      <c r="J13" s="467"/>
     </row>
     <row r="14" spans="2:10">
       <c r="C14" s="87" t="s">
@@ -16838,17 +16694,17 @@
       </c>
       <c r="G14" s="76">
         <f>$G13</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H14" s="77">
         <f>$H13</f>
         <v>0</v>
       </c>
-      <c r="I14" s="458">
+      <c r="I14" s="466">
         <f t="shared" ref="I14:I17" si="0">$I13</f>
         <v>3</v>
       </c>
-      <c r="J14" s="459"/>
+      <c r="J14" s="467"/>
     </row>
     <row r="15" spans="2:10">
       <c r="C15" s="87" t="s">
@@ -16868,17 +16724,17 @@
       </c>
       <c r="G15" s="76">
         <f>$G14</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H15" s="77">
         <f>$H14</f>
         <v>0</v>
       </c>
-      <c r="I15" s="458">
+      <c r="I15" s="466">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J15" s="459"/>
+      <c r="J15" s="467"/>
     </row>
     <row r="16" spans="2:10">
       <c r="C16" s="87" t="s">
@@ -16898,17 +16754,17 @@
       </c>
       <c r="G16" s="76">
         <f>$G15</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H16" s="77">
         <f>$H15</f>
         <v>0</v>
       </c>
-      <c r="I16" s="458">
+      <c r="I16" s="466">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J16" s="459"/>
+      <c r="J16" s="467"/>
     </row>
     <row r="17" spans="3:10" ht="15.75" thickBot="1">
       <c r="C17" s="88" t="s">
@@ -16928,17 +16784,17 @@
       </c>
       <c r="G17" s="78">
         <f>$G16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="79">
         <f>$H16</f>
         <v>0</v>
       </c>
-      <c r="I17" s="458">
+      <c r="I17" s="466">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J17" s="459"/>
+      <c r="J17" s="467"/>
     </row>
     <row r="18" spans="3:10">
       <c r="C18" s="86" t="s">
@@ -16958,17 +16814,17 @@
       </c>
       <c r="G18" s="74">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18" s="75">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="477">
+      <c r="I18" s="485">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J18" s="478"/>
+      <c r="J18" s="486"/>
     </row>
     <row r="19" spans="3:10" ht="27" customHeight="1">
       <c r="C19" s="94" t="s">
@@ -16989,10 +16845,10 @@
       <c r="H19" s="147">
         <v>60</v>
       </c>
-      <c r="I19" s="480">
+      <c r="I19" s="488">
         <v>100</v>
       </c>
-      <c r="J19" s="481"/>
+      <c r="J19" s="489"/>
     </row>
     <row r="20" spans="3:10" ht="31.5" customHeight="1" thickBot="1">
       <c r="C20" s="89" t="s">
@@ -17012,32 +16868,32 @@
       </c>
       <c r="G20" s="85">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H20" s="85">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I20" s="482">
+      <c r="I20" s="490">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J20" s="483">
+      <c r="J20" s="491">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:10" ht="48" customHeight="1" thickBot="1">
-      <c r="C21" s="484" t="s">
+      <c r="C21" s="492" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="484"/>
-      <c r="E21" s="484"/>
-      <c r="F21" s="484"/>
-      <c r="G21" s="484"/>
+      <c r="D21" s="492"/>
+      <c r="E21" s="492"/>
+      <c r="F21" s="492"/>
+      <c r="G21" s="492"/>
       <c r="H21" s="90">
         <f>SUM(D20:H20)</f>
-        <v>1.083</v>
+        <v>0.78299999999999992</v>
       </c>
       <c r="I21" s="91" t="s">
         <v>93</v>
@@ -17048,13 +16904,13 @@
       </c>
     </row>
     <row r="22" spans="3:10" ht="22.5" customHeight="1" thickBot="1">
-      <c r="C22" s="484" t="s">
+      <c r="C22" s="492" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="484"/>
-      <c r="E22" s="484"/>
-      <c r="F22" s="484"/>
-      <c r="G22" s="484"/>
+      <c r="D22" s="492"/>
+      <c r="E22" s="492"/>
+      <c r="F22" s="492"/>
+      <c r="G22" s="492"/>
       <c r="H22" s="92">
         <v>0.8</v>
       </c>
@@ -17066,16 +16922,16 @@
       </c>
     </row>
     <row r="23" spans="3:10" ht="45" customHeight="1" thickBot="1">
-      <c r="C23" s="484" t="s">
+      <c r="C23" s="492" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="484"/>
-      <c r="E23" s="484"/>
-      <c r="F23" s="484"/>
-      <c r="G23" s="484"/>
+      <c r="D23" s="492"/>
+      <c r="E23" s="492"/>
+      <c r="F23" s="492"/>
+      <c r="G23" s="492"/>
       <c r="H23" s="93">
         <f>0.8*H21</f>
-        <v>0.86640000000000006</v>
+        <v>0.62639999999999996</v>
       </c>
       <c r="I23" s="91" t="s">
         <v>94</v>
@@ -17086,17 +16942,17 @@
       </c>
     </row>
     <row r="24" spans="3:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="C24" s="479" t="s">
+      <c r="C24" s="487" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="479"/>
-      <c r="E24" s="479"/>
-      <c r="F24" s="479"/>
-      <c r="G24" s="479"/>
-      <c r="H24" s="479"/>
+      <c r="D24" s="487"/>
+      <c r="E24" s="487"/>
+      <c r="F24" s="487"/>
+      <c r="G24" s="487"/>
+      <c r="H24" s="487"/>
       <c r="I24" s="111">
         <f>ROUNDUP(H23+J23,2)</f>
-        <v>1.47</v>
+        <v>1.23</v>
       </c>
       <c r="J24" s="112"/>
     </row>
@@ -17152,7 +17008,7 @@
   </sheetPr>
   <dimension ref="B1:K41"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18:J18"/>
     </sheetView>
   </sheetViews>
@@ -17224,15 +17080,15 @@
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="1"/>
-      <c r="C8" s="506" t="s">
+      <c r="C8" s="514" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="507"/>
-      <c r="E8" s="510" t="s">
+      <c r="D8" s="515"/>
+      <c r="E8" s="518" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="510"/>
-      <c r="G8" s="510"/>
+      <c r="F8" s="518"/>
+      <c r="G8" s="518"/>
       <c r="H8" s="154" t="s">
         <v>181</v>
       </c>
@@ -17242,14 +17098,14 @@
       <c r="J8" s="154" t="s">
         <v>175</v>
       </c>
-      <c r="K8" s="514" t="s">
+      <c r="K8" s="522" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="30.75" thickBot="1">
       <c r="B9" s="1"/>
-      <c r="C9" s="508"/>
-      <c r="D9" s="509"/>
+      <c r="C9" s="516"/>
+      <c r="D9" s="517"/>
       <c r="E9" s="176" t="s">
         <v>179</v>
       </c>
@@ -17268,18 +17124,18 @@
       <c r="J9" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="515"/>
+      <c r="K9" s="523"/>
     </row>
     <row r="10" spans="2:11" ht="19.5" customHeight="1">
       <c r="B10" s="1"/>
-      <c r="C10" s="516" t="s">
+      <c r="C10" s="524" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="406"/>
-      <c r="E10" s="510">
+      <c r="D10" s="414"/>
+      <c r="E10" s="518">
         <v>20</v>
       </c>
-      <c r="F10" s="510"/>
+      <c r="F10" s="518"/>
       <c r="G10" s="154">
         <v>10</v>
       </c>
@@ -17299,15 +17155,15 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" customHeight="1" thickBot="1">
       <c r="B11" s="1"/>
-      <c r="C11" s="517" t="s">
+      <c r="C11" s="525" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="333"/>
-      <c r="E11" s="518">
+      <c r="D11" s="341"/>
+      <c r="E11" s="526">
         <f>(E10/$K10)*100</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="F11" s="519"/>
+      <c r="F11" s="527"/>
       <c r="G11" s="177">
         <f>(G10/$K10)*100</f>
         <v>6.666666666666667</v>
@@ -17336,33 +17192,33 @@
     </row>
     <row r="13" spans="2:11" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="14" spans="2:11" ht="21.75" thickBot="1">
-      <c r="C14" s="511" t="s">
+      <c r="C14" s="519" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="512"/>
-      <c r="E14" s="512"/>
-      <c r="F14" s="512"/>
-      <c r="G14" s="512"/>
-      <c r="H14" s="512"/>
-      <c r="I14" s="512"/>
-      <c r="J14" s="513"/>
+      <c r="D14" s="520"/>
+      <c r="E14" s="520"/>
+      <c r="F14" s="520"/>
+      <c r="G14" s="520"/>
+      <c r="H14" s="520"/>
+      <c r="I14" s="520"/>
+      <c r="J14" s="521"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1">
-      <c r="C15" s="501" t="s">
+      <c r="C15" s="509" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="502"/>
-      <c r="E15" s="502"/>
-      <c r="F15" s="502"/>
-      <c r="G15" s="502"/>
-      <c r="H15" s="503"/>
-      <c r="I15" s="491" t="s">
+      <c r="D15" s="510"/>
+      <c r="E15" s="510"/>
+      <c r="F15" s="510"/>
+      <c r="G15" s="510"/>
+      <c r="H15" s="511"/>
+      <c r="I15" s="499" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="492"/>
+      <c r="J15" s="500"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1">
-      <c r="C16" s="504" t="s">
+      <c r="C16" s="512" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="173"/>
@@ -17374,11 +17230,11 @@
       <c r="H16" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="493"/>
-      <c r="J16" s="494"/>
+      <c r="I16" s="501"/>
+      <c r="J16" s="502"/>
     </row>
     <row r="17" spans="3:10" ht="45.75" customHeight="1" thickBot="1">
-      <c r="C17" s="505"/>
+      <c r="C17" s="513"/>
       <c r="D17" s="150" t="s">
         <v>77</v>
       </c>
@@ -17394,10 +17250,10 @@
       <c r="H17" s="181" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="495" t="s">
+      <c r="I17" s="503" t="s">
         <v>91</v>
       </c>
-      <c r="J17" s="496"/>
+      <c r="J17" s="504"/>
     </row>
     <row r="18" spans="3:10">
       <c r="C18" s="152" t="s">
@@ -17417,17 +17273,17 @@
       </c>
       <c r="G18" s="154">
         <f>'CO_attain_MicroP_PR-TW_ESE'!C94</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18" s="155">
         <f>'CO_attainment for ESEBoard Exam'!C92</f>
         <v>0</v>
       </c>
-      <c r="I18" s="485">
+      <c r="I18" s="493">
         <f>'CO_attainment for Indirect'!C92</f>
         <v>3</v>
       </c>
-      <c r="J18" s="486"/>
+      <c r="J18" s="494"/>
     </row>
     <row r="19" spans="3:10">
       <c r="C19" s="156" t="s">
@@ -17447,17 +17303,17 @@
       </c>
       <c r="G19" s="158">
         <f>$G18</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19" s="159">
         <f>$H18</f>
         <v>0</v>
       </c>
-      <c r="I19" s="497">
+      <c r="I19" s="505">
         <f>$I18</f>
         <v>3</v>
       </c>
-      <c r="J19" s="498"/>
+      <c r="J19" s="506"/>
     </row>
     <row r="20" spans="3:10">
       <c r="C20" s="156" t="s">
@@ -17477,17 +17333,17 @@
       </c>
       <c r="G20" s="158">
         <f>$G19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20" s="159">
         <f>$H19</f>
         <v>0</v>
       </c>
-      <c r="I20" s="497">
+      <c r="I20" s="505">
         <f t="shared" ref="I20:I23" si="0">$I19</f>
         <v>3</v>
       </c>
-      <c r="J20" s="498"/>
+      <c r="J20" s="506"/>
     </row>
     <row r="21" spans="3:10">
       <c r="C21" s="156" t="s">
@@ -17507,17 +17363,17 @@
       </c>
       <c r="G21" s="158">
         <f>$G20</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H21" s="159">
         <f>$H20</f>
         <v>0</v>
       </c>
-      <c r="I21" s="497">
+      <c r="I21" s="505">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J21" s="498"/>
+      <c r="J21" s="506"/>
     </row>
     <row r="22" spans="3:10">
       <c r="C22" s="156" t="s">
@@ -17537,17 +17393,17 @@
       </c>
       <c r="G22" s="158">
         <f>$G21</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="159">
         <f>$H21</f>
         <v>0</v>
       </c>
-      <c r="I22" s="497">
+      <c r="I22" s="505">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J22" s="498"/>
+      <c r="J22" s="506"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1">
       <c r="C23" s="160" t="s">
@@ -17567,17 +17423,17 @@
       </c>
       <c r="G23" s="162">
         <f>$G22</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H23" s="163">
         <f>$H22</f>
         <v>0</v>
       </c>
-      <c r="I23" s="497">
+      <c r="I23" s="505">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J23" s="498"/>
+      <c r="J23" s="506"/>
     </row>
     <row r="24" spans="3:10">
       <c r="C24" s="152" t="s">
@@ -17597,17 +17453,17 @@
       </c>
       <c r="G24" s="154">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H24" s="155">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="485">
+      <c r="I24" s="493">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J24" s="486"/>
+      <c r="J24" s="494"/>
     </row>
     <row r="25" spans="3:10" ht="30">
       <c r="C25" s="164" t="s">
@@ -17633,10 +17489,10 @@
         <f>J11</f>
         <v>46.666666666666664</v>
       </c>
-      <c r="I25" s="487">
+      <c r="I25" s="495">
         <v>100</v>
       </c>
-      <c r="J25" s="488"/>
+      <c r="J25" s="496"/>
     </row>
     <row r="26" spans="3:10" ht="30.75" thickBot="1">
       <c r="C26" s="165" t="s">
@@ -17656,29 +17512,29 @@
       </c>
       <c r="G26" s="184">
         <f t="shared" si="2"/>
-        <v>0.49999999999999994</v>
+        <v>0</v>
       </c>
       <c r="H26" s="184">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I26" s="489">
+      <c r="I26" s="497">
         <f>I24*I25/100</f>
         <v>3</v>
       </c>
-      <c r="J26" s="490"/>
+      <c r="J26" s="498"/>
     </row>
     <row r="27" spans="3:10" ht="30" customHeight="1" thickBot="1">
-      <c r="C27" s="499" t="s">
+      <c r="C27" s="507" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="499"/>
-      <c r="E27" s="499"/>
-      <c r="F27" s="499"/>
-      <c r="G27" s="499"/>
+      <c r="D27" s="507"/>
+      <c r="E27" s="507"/>
+      <c r="F27" s="507"/>
+      <c r="G27" s="507"/>
       <c r="H27" s="185">
         <f>SUM(D26:H26)</f>
-        <v>1.444</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="I27" s="167" t="s">
         <v>93</v>
@@ -17689,13 +17545,13 @@
       </c>
     </row>
     <row r="28" spans="3:10" ht="15.75" thickBot="1">
-      <c r="C28" s="499" t="s">
+      <c r="C28" s="507" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="499"/>
-      <c r="E28" s="499"/>
-      <c r="F28" s="499"/>
-      <c r="G28" s="499"/>
+      <c r="D28" s="507"/>
+      <c r="E28" s="507"/>
+      <c r="F28" s="507"/>
+      <c r="G28" s="507"/>
       <c r="H28" s="168">
         <v>0.8</v>
       </c>
@@ -17707,16 +17563,16 @@
       </c>
     </row>
     <row r="29" spans="3:10" ht="62.25" customHeight="1" thickBot="1">
-      <c r="C29" s="499" t="s">
+      <c r="C29" s="507" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="499"/>
-      <c r="E29" s="499"/>
-      <c r="F29" s="499"/>
-      <c r="G29" s="499"/>
+      <c r="D29" s="507"/>
+      <c r="E29" s="507"/>
+      <c r="F29" s="507"/>
+      <c r="G29" s="507"/>
       <c r="H29" s="185">
         <f>0.8*H27</f>
-        <v>1.1552</v>
+        <v>0.75519999999999998</v>
       </c>
       <c r="I29" s="167" t="s">
         <v>94</v>
@@ -17727,17 +17583,17 @@
       </c>
     </row>
     <row r="30" spans="3:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="C30" s="500" t="s">
+      <c r="C30" s="508" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="500"/>
-      <c r="E30" s="500"/>
-      <c r="F30" s="500"/>
-      <c r="G30" s="500"/>
-      <c r="H30" s="500"/>
+      <c r="D30" s="508"/>
+      <c r="E30" s="508"/>
+      <c r="F30" s="508"/>
+      <c r="G30" s="508"/>
+      <c r="H30" s="508"/>
       <c r="I30" s="170">
         <f>ROUNDUP(H29+J29,2)</f>
-        <v>1.76</v>
+        <v>1.36</v>
       </c>
       <c r="J30" s="171"/>
     </row>
@@ -17808,7 +17664,7 @@
   </sheetPr>
   <dimension ref="B1:M23"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -17873,31 +17729,31 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="16.5" thickBot="1">
-      <c r="B8" s="311" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="314" t="s">
+      <c r="B8" s="319" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="322" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="315"/>
-      <c r="E8" s="320" t="s">
+      <c r="D8" s="323"/>
+      <c r="E8" s="328" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="321"/>
-      <c r="G8" s="321"/>
-      <c r="H8" s="321"/>
-      <c r="I8" s="321"/>
-      <c r="J8" s="321"/>
-      <c r="K8" s="322"/>
-      <c r="L8" s="320" t="s">
+      <c r="F8" s="329"/>
+      <c r="G8" s="329"/>
+      <c r="H8" s="329"/>
+      <c r="I8" s="329"/>
+      <c r="J8" s="329"/>
+      <c r="K8" s="330"/>
+      <c r="L8" s="328" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="321"/>
+      <c r="M8" s="329"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B9" s="312"/>
-      <c r="C9" s="316"/>
-      <c r="D9" s="317"/>
+      <c r="B9" s="320"/>
+      <c r="C9" s="324"/>
+      <c r="D9" s="325"/>
       <c r="E9" s="118" t="s">
         <v>98</v>
       </c>
@@ -17927,9 +17783,9 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="81" customHeight="1" thickBot="1">
-      <c r="B10" s="313"/>
-      <c r="C10" s="318"/>
-      <c r="D10" s="319"/>
+      <c r="B10" s="321"/>
+      <c r="C10" s="326"/>
+      <c r="D10" s="327"/>
       <c r="E10" s="119" t="s">
         <v>133</v>
       </c>
@@ -17973,15 +17829,15 @@
       </c>
       <c r="E11" s="125">
         <f>'PO Set Target attain level'!E19</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="125">
         <f>'PO Set Target attain level'!F19</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="125">
         <f>'PO Set Target attain level'!G19</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" s="125">
         <f>'PO Set Target attain level'!H19</f>
@@ -17993,19 +17849,19 @@
       </c>
       <c r="J11" s="125">
         <f>'PO Set Target attain level'!J19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="125">
         <f>'PO Set Target attain level'!K19</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" s="125">
         <f>'PO Set Target attain level'!L19</f>
-        <v>2</v>
-      </c>
-      <c r="M11" s="125" t="str">
+        <v>1</v>
+      </c>
+      <c r="M11" s="125">
         <f>'PO Set Target attain level'!M19</f>
-        <v>-</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="24.75" thickBot="1">
@@ -18023,39 +17879,39 @@
       </c>
       <c r="E12" s="125">
         <f>'PO Set Target attain level'!E20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="125">
         <f>'PO Set Target attain level'!F20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="125">
         <f>'PO Set Target attain level'!G20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="125">
         <f>'PO Set Target attain level'!H20</f>
-        <v>2</v>
-      </c>
-      <c r="I12" s="125">
+        <v>1</v>
+      </c>
+      <c r="I12" s="125" t="str">
         <f>'PO Set Target attain level'!I20</f>
-        <v>2</v>
+        <v>-</v>
       </c>
       <c r="J12" s="125">
         <f>'PO Set Target attain level'!J20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="125">
         <f>'PO Set Target attain level'!K20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" s="125">
         <f>'PO Set Target attain level'!L20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="125">
         <f>'PO Set Target attain level'!M20</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="24.75" thickBot="1">
@@ -18073,7 +17929,7 @@
       </c>
       <c r="E13" s="125">
         <f>'PO Set Target attain level'!E21</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="125">
         <f>'PO Set Target attain level'!F21</f>
@@ -18081,11 +17937,11 @@
       </c>
       <c r="G13" s="125">
         <f>'PO Set Target attain level'!G21</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="125" t="str">
+        <v>2</v>
+      </c>
+      <c r="H13" s="125">
         <f>'PO Set Target attain level'!H21</f>
-        <v>-</v>
+        <v>1</v>
       </c>
       <c r="I13" s="125">
         <f>'PO Set Target attain level'!I21</f>
@@ -18097,15 +17953,15 @@
       </c>
       <c r="K13" s="125">
         <f>'PO Set Target attain level'!K21</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L13" s="125">
         <f>'PO Set Target attain level'!L21</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="125" t="str">
+        <v>2</v>
+      </c>
+      <c r="M13" s="125">
         <f>'PO Set Target attain level'!M21</f>
-        <v>-</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1">
@@ -18131,19 +17987,19 @@
       </c>
       <c r="G14" s="125">
         <f>'PO Set Target attain level'!G22</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14" s="125">
         <f>'PO Set Target attain level'!H22</f>
         <v>2</v>
       </c>
-      <c r="I14" s="125">
+      <c r="I14" s="125" t="str">
         <f>'PO Set Target attain level'!I22</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="J14" s="125">
         <f>'PO Set Target attain level'!J22</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="125">
         <f>'PO Set Target attain level'!K22</f>
@@ -18151,11 +18007,11 @@
       </c>
       <c r="L14" s="125">
         <f>'PO Set Target attain level'!L22</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M14" s="125">
         <f>'PO Set Target attain level'!M22</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1">
@@ -18173,11 +18029,11 @@
       </c>
       <c r="E15" s="125">
         <f>'PO Set Target attain level'!E23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="125">
         <f>'PO Set Target attain level'!F23</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="125">
         <f>'PO Set Target attain level'!G23</f>
@@ -18185,54 +18041,54 @@
       </c>
       <c r="H15" s="125">
         <f>'PO Set Target attain level'!H23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="125">
         <f>'PO Set Target attain level'!I23</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="125">
         <f>'PO Set Target attain level'!J23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15" s="125">
         <f>'PO Set Target attain level'!K23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" s="125">
         <f>'PO Set Target attain level'!L23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M15" s="125">
         <f>'PO Set Target attain level'!M23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B16" s="520" t="s">
+      <c r="B16" s="528" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="521"/>
-      <c r="D16" s="522"/>
+      <c r="C16" s="529"/>
+      <c r="D16" s="530"/>
       <c r="E16" s="146">
         <f t="shared" ref="E16:M16" si="0">ROUNDUP(AVERAGE(E11:E15),2)</f>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="F16" s="146">
         <f t="shared" si="0"/>
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
       <c r="G16" s="146">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>1.8</v>
       </c>
       <c r="H16" s="146">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="I16" s="146">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="146">
         <f t="shared" si="0"/>
@@ -18240,92 +18096,92 @@
       </c>
       <c r="K16" s="146">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="L16" s="146">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M16" s="146">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B17" s="523" t="s">
+      <c r="B17" s="531" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="524"/>
-      <c r="D17" s="525"/>
+      <c r="C17" s="532"/>
+      <c r="D17" s="533"/>
       <c r="E17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*E16)/3,2)</f>
-        <v>1.65</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*F16)/3,2)</f>
-        <v>1.41</v>
+        <v>0.73</v>
       </c>
       <c r="G17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*G16)/3,2)</f>
-        <v>1.65</v>
+        <v>0.82000000000000006</v>
       </c>
       <c r="H17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*H16)/3,2)</f>
-        <v>0.88</v>
+        <v>0.64</v>
       </c>
       <c r="I17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*I16)/3,2)</f>
-        <v>0.88</v>
+        <v>0.46</v>
       </c>
       <c r="J17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*J16)/3,2)</f>
-        <v>1.41</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*K16)/3,2)</f>
-        <v>1.65</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="L17" s="128" t="s">
         <v>187</v>
       </c>
       <c r="M17" s="128">
         <f>ROUNDUP(('Overall CO attainment'!I30*M16)/3,2)</f>
-        <v>0.59</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B18" s="523" t="s">
+      <c r="B18" s="531" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="524"/>
-      <c r="D18" s="525"/>
+      <c r="C18" s="532"/>
+      <c r="D18" s="533"/>
       <c r="E18" s="128">
         <f>ROUNDUP((E17/3)*100,2)</f>
-        <v>55</v>
+        <v>36.339999999999996</v>
       </c>
       <c r="F18" s="128">
         <f t="shared" ref="F18:M18" si="1">ROUNDUP((F17/3)*100,2)</f>
-        <v>47</v>
+        <v>24.34</v>
       </c>
       <c r="G18" s="128">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>27.34</v>
       </c>
       <c r="H18" s="128">
         <f t="shared" si="1"/>
-        <v>29.34</v>
+        <v>21.34</v>
       </c>
       <c r="I18" s="128">
         <f t="shared" si="1"/>
-        <v>29.34</v>
+        <v>15.34</v>
       </c>
       <c r="J18" s="128">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>36.339999999999996</v>
       </c>
       <c r="K18" s="128">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>36.339999999999996</v>
       </c>
       <c r="L18" s="128" t="e">
         <f t="shared" si="1"/>
@@ -18333,7 +18189,7 @@
       </c>
       <c r="M18" s="128">
         <f t="shared" si="1"/>
-        <v>19.670000000000002</v>
+        <v>36.339999999999996</v>
       </c>
     </row>
     <row r="22" spans="2:13">

</xml_diff>